<commit_message>
docs: add main descr for the final project
</commit_message>
<xml_diff>
--- a/yandex-samokat/yandex-samokat (mobile version).xlsx
+++ b/yandex-samokat/yandex-samokat (mobile version).xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vladefremov/Documents/Тестирование/ЯндексПрактикум/Practicum_projects/yandex-samokat/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63A9CFAC-B177-5B49-870F-91E00C85DDDE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58FC8B01-0CF7-4D45-ACD7-C380FD97E094}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{D0BC9613-3873-3245-A71C-614316A097B5}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{D0BC9613-3873-3245-A71C-614316A097B5}"/>
   </bookViews>
   <sheets>
     <sheet name="Тест-кейсы" sheetId="1" r:id="rId1"/>
     <sheet name="Баг-репорты" sheetId="3" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="410" uniqueCount="184">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="409" uniqueCount="184">
   <si>
     <t>"Ок" - Первая заглавная, без выделения</t>
   </si>
@@ -2210,7 +2210,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -2251,24 +2251,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2289,17 +2275,22 @@
     <xf numFmtId="0" fontId="8" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2777,18 +2768,18 @@
   </sheetPr>
   <dimension ref="A1:Y998"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E59" sqref="E59"/>
+      <selection pane="bottomLeft" activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="15.19921875" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9.796875" style="31" customWidth="1"/>
+    <col min="1" max="1" width="9.796875" style="22" customWidth="1"/>
     <col min="2" max="2" width="37.3984375" customWidth="1"/>
     <col min="3" max="3" width="47.796875" customWidth="1"/>
     <col min="4" max="4" width="63.796875" customWidth="1"/>
-    <col min="5" max="5" width="39" style="31" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="39" style="22" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="25.796875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12.59765625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="25.796875" bestFit="1" customWidth="1"/>
@@ -2796,28 +2787,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:25" ht="35" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="15" t="s">
         <v>176</v>
       </c>
-      <c r="B1" s="19" t="s">
+      <c r="B1" s="15" t="s">
         <v>175</v>
       </c>
-      <c r="C1" s="19" t="s">
+      <c r="C1" s="15" t="s">
         <v>174</v>
       </c>
-      <c r="D1" s="19" t="s">
+      <c r="D1" s="15" t="s">
         <v>173</v>
       </c>
-      <c r="E1" s="19" t="s">
+      <c r="E1" s="15" t="s">
         <v>172</v>
       </c>
-      <c r="F1" s="19" t="s">
+      <c r="F1" s="15" t="s">
         <v>171</v>
       </c>
-      <c r="G1" s="19" t="s">
+      <c r="G1" s="15" t="s">
         <v>170</v>
       </c>
-      <c r="H1" s="19" t="s">
+      <c r="H1" s="15" t="s">
         <v>169</v>
       </c>
       <c r="I1" s="2"/>
@@ -2839,16 +2830,16 @@
       <c r="Y1" s="1"/>
     </row>
     <row r="2" spans="1:25" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="18" t="s">
+      <c r="A2" s="26" t="s">
         <v>168</v>
       </c>
-      <c r="B2" s="20"/>
-      <c r="C2" s="20"/>
-      <c r="D2" s="20"/>
-      <c r="E2" s="20"/>
-      <c r="F2" s="20"/>
-      <c r="G2" s="20"/>
-      <c r="H2" s="21"/>
+      <c r="B2" s="27"/>
+      <c r="C2" s="27"/>
+      <c r="D2" s="27"/>
+      <c r="E2" s="27"/>
+      <c r="F2" s="27"/>
+      <c r="G2" s="27"/>
+      <c r="H2" s="28"/>
       <c r="I2" s="5"/>
       <c r="J2" s="4"/>
       <c r="K2" s="4"/>
@@ -2868,16 +2859,16 @@
       <c r="Y2" s="4"/>
     </row>
     <row r="3" spans="1:25" ht="34.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="16" t="s">
+      <c r="A3" s="23" t="s">
         <v>167</v>
       </c>
-      <c r="B3" s="15"/>
-      <c r="C3" s="15"/>
-      <c r="D3" s="15"/>
-      <c r="E3" s="15"/>
-      <c r="F3" s="15"/>
-      <c r="G3" s="15"/>
-      <c r="H3" s="14"/>
+      <c r="B3" s="24"/>
+      <c r="C3" s="24"/>
+      <c r="D3" s="24"/>
+      <c r="E3" s="24"/>
+      <c r="F3" s="24"/>
+      <c r="G3" s="24"/>
+      <c r="H3" s="25"/>
       <c r="I3" s="5"/>
       <c r="J3" s="4"/>
       <c r="K3" s="4"/>
@@ -2953,9 +2944,7 @@
       <c r="E5" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="F5" s="8" t="s">
-        <v>70</v>
-      </c>
+      <c r="F5" s="8"/>
       <c r="G5" s="9" t="s">
         <v>69</v>
       </c>
@@ -3168,7 +3157,7 @@
       <c r="G10" s="9" t="s">
         <v>74</v>
       </c>
-      <c r="H10" s="17"/>
+      <c r="H10" s="14"/>
       <c r="I10" s="2"/>
       <c r="J10" s="1"/>
       <c r="K10" s="1"/>
@@ -3209,7 +3198,7 @@
       <c r="G11" s="9" t="s">
         <v>74</v>
       </c>
-      <c r="H11" s="17"/>
+      <c r="H11" s="14"/>
       <c r="I11" s="2"/>
       <c r="J11" s="1"/>
       <c r="K11" s="1"/>
@@ -3293,7 +3282,7 @@
       <c r="G13" s="9" t="s">
         <v>74</v>
       </c>
-      <c r="H13" s="17"/>
+      <c r="H13" s="14"/>
       <c r="I13" s="2"/>
       <c r="J13" s="1"/>
       <c r="K13" s="1"/>
@@ -3377,7 +3366,7 @@
       <c r="G15" s="9" t="s">
         <v>74</v>
       </c>
-      <c r="H15" s="17"/>
+      <c r="H15" s="14"/>
       <c r="I15" s="2"/>
       <c r="J15" s="1"/>
       <c r="K15" s="1"/>
@@ -3418,7 +3407,7 @@
       <c r="G16" s="9" t="s">
         <v>74</v>
       </c>
-      <c r="H16" s="17"/>
+      <c r="H16" s="14"/>
       <c r="I16" s="2"/>
       <c r="J16" s="1"/>
       <c r="K16" s="1"/>
@@ -3459,7 +3448,7 @@
       <c r="G17" s="9" t="s">
         <v>74</v>
       </c>
-      <c r="H17" s="17"/>
+      <c r="H17" s="14"/>
       <c r="I17" s="2"/>
       <c r="J17" s="1"/>
       <c r="K17" s="1"/>
@@ -3500,7 +3489,7 @@
       <c r="G18" s="9" t="s">
         <v>74</v>
       </c>
-      <c r="H18" s="17"/>
+      <c r="H18" s="14"/>
       <c r="I18" s="2"/>
       <c r="J18" s="1"/>
       <c r="K18" s="1"/>
@@ -3541,7 +3530,7 @@
       <c r="G19" s="9" t="s">
         <v>74</v>
       </c>
-      <c r="H19" s="17"/>
+      <c r="H19" s="14"/>
       <c r="I19" s="2"/>
       <c r="J19" s="1"/>
       <c r="K19" s="1"/>
@@ -3582,7 +3571,7 @@
       <c r="G20" s="9" t="s">
         <v>74</v>
       </c>
-      <c r="H20" s="17"/>
+      <c r="H20" s="14"/>
       <c r="I20" s="2"/>
       <c r="J20" s="1"/>
       <c r="K20" s="1"/>
@@ -3623,7 +3612,7 @@
       <c r="G21" s="9" t="s">
         <v>74</v>
       </c>
-      <c r="H21" s="17"/>
+      <c r="H21" s="14"/>
       <c r="I21" s="2"/>
       <c r="J21" s="1"/>
       <c r="K21" s="1"/>
@@ -3643,16 +3632,16 @@
       <c r="Y21" s="1"/>
     </row>
     <row r="22" spans="1:25" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="16" t="s">
+      <c r="A22" s="23" t="s">
         <v>129</v>
       </c>
-      <c r="B22" s="15"/>
-      <c r="C22" s="15"/>
-      <c r="D22" s="15"/>
-      <c r="E22" s="15"/>
-      <c r="F22" s="15"/>
-      <c r="G22" s="15"/>
-      <c r="H22" s="14"/>
+      <c r="B22" s="24"/>
+      <c r="C22" s="24"/>
+      <c r="D22" s="24"/>
+      <c r="E22" s="24"/>
+      <c r="F22" s="24"/>
+      <c r="G22" s="24"/>
+      <c r="H22" s="25"/>
       <c r="I22" s="2"/>
       <c r="J22" s="1"/>
       <c r="K22" s="1"/>
@@ -3799,16 +3788,16 @@
       <c r="Y25" s="4"/>
     </row>
     <row r="26" spans="1:25" ht="34.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="16" t="s">
+      <c r="A26" s="23" t="s">
         <v>122</v>
       </c>
-      <c r="B26" s="15"/>
-      <c r="C26" s="15"/>
-      <c r="D26" s="15"/>
-      <c r="E26" s="15"/>
-      <c r="F26" s="15"/>
-      <c r="G26" s="15"/>
-      <c r="H26" s="14"/>
+      <c r="B26" s="24"/>
+      <c r="C26" s="24"/>
+      <c r="D26" s="24"/>
+      <c r="E26" s="24"/>
+      <c r="F26" s="24"/>
+      <c r="G26" s="24"/>
+      <c r="H26" s="25"/>
       <c r="I26" s="2"/>
       <c r="J26" s="1"/>
       <c r="K26" s="1"/>
@@ -3871,28 +3860,28 @@
       <c r="Y27" s="4"/>
     </row>
     <row r="28" spans="1:25" ht="96" x14ac:dyDescent="0.2">
-      <c r="A28" s="28">
+      <c r="A28" s="13">
         <v>23</v>
       </c>
-      <c r="B28" s="29" t="s">
+      <c r="B28" s="8" t="s">
         <v>120</v>
       </c>
-      <c r="C28" s="29" t="s">
+      <c r="C28" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="D28" s="29" t="s">
+      <c r="D28" s="8" t="s">
         <v>114</v>
       </c>
-      <c r="E28" s="29" t="s">
+      <c r="E28" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="F28" s="29" t="s">
+      <c r="F28" s="8" t="s">
         <v>70</v>
       </c>
-      <c r="G28" s="30" t="s">
+      <c r="G28" s="9" t="s">
         <v>69</v>
       </c>
-      <c r="H28" s="30" t="s">
+      <c r="H28" s="9" t="s">
         <v>39</v>
       </c>
       <c r="I28" s="2"/>
@@ -3914,28 +3903,28 @@
       <c r="Y28" s="1"/>
     </row>
     <row r="29" spans="1:25" ht="96" x14ac:dyDescent="0.2">
-      <c r="A29" s="28">
+      <c r="A29" s="13">
         <v>24</v>
       </c>
-      <c r="B29" s="29" t="s">
+      <c r="B29" s="8" t="s">
         <v>119</v>
       </c>
-      <c r="C29" s="29" t="s">
+      <c r="C29" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="D29" s="29" t="s">
+      <c r="D29" s="8" t="s">
         <v>112</v>
       </c>
-      <c r="E29" s="29" t="s">
+      <c r="E29" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="F29" s="29" t="s">
+      <c r="F29" s="8" t="s">
         <v>70</v>
       </c>
-      <c r="G29" s="30" t="s">
+      <c r="G29" s="9" t="s">
         <v>69</v>
       </c>
-      <c r="H29" s="30" t="s">
+      <c r="H29" s="9" t="s">
         <v>39</v>
       </c>
       <c r="I29" s="2"/>
@@ -3957,28 +3946,28 @@
       <c r="Y29" s="1"/>
     </row>
     <row r="30" spans="1:25" ht="105" x14ac:dyDescent="0.2">
-      <c r="A30" s="28">
+      <c r="A30" s="13">
         <v>25</v>
       </c>
-      <c r="B30" s="29" t="s">
+      <c r="B30" s="8" t="s">
         <v>118</v>
       </c>
-      <c r="C30" s="29" t="s">
+      <c r="C30" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="D30" s="29" t="s">
+      <c r="D30" s="8" t="s">
         <v>117</v>
       </c>
-      <c r="E30" s="29" t="s">
+      <c r="E30" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="F30" s="29" t="s">
+      <c r="F30" s="8" t="s">
         <v>70</v>
       </c>
-      <c r="G30" s="30" t="s">
+      <c r="G30" s="9" t="s">
         <v>69</v>
       </c>
-      <c r="H30" s="30" t="s">
+      <c r="H30" s="9" t="s">
         <v>39</v>
       </c>
       <c r="I30" s="2"/>
@@ -4043,28 +4032,28 @@
       <c r="Y31" s="1"/>
     </row>
     <row r="32" spans="1:25" ht="96" x14ac:dyDescent="0.2">
-      <c r="A32" s="28">
+      <c r="A32" s="13">
         <v>27</v>
       </c>
-      <c r="B32" s="29" t="s">
+      <c r="B32" s="8" t="s">
         <v>115</v>
       </c>
-      <c r="C32" s="29" t="s">
+      <c r="C32" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="D32" s="29" t="s">
+      <c r="D32" s="8" t="s">
         <v>114</v>
       </c>
-      <c r="E32" s="29" t="s">
+      <c r="E32" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="F32" s="29" t="s">
+      <c r="F32" s="8" t="s">
         <v>70</v>
       </c>
-      <c r="G32" s="30" t="s">
+      <c r="G32" s="9" t="s">
         <v>69</v>
       </c>
-      <c r="H32" s="30" t="s">
+      <c r="H32" s="9" t="s">
         <v>32</v>
       </c>
       <c r="I32" s="2"/>
@@ -4086,28 +4075,28 @@
       <c r="Y32" s="1"/>
     </row>
     <row r="33" spans="1:25" ht="96" x14ac:dyDescent="0.2">
-      <c r="A33" s="28">
+      <c r="A33" s="13">
         <v>28</v>
       </c>
-      <c r="B33" s="29" t="s">
+      <c r="B33" s="8" t="s">
         <v>113</v>
       </c>
-      <c r="C33" s="29" t="s">
+      <c r="C33" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="D33" s="29" t="s">
+      <c r="D33" s="8" t="s">
         <v>112</v>
       </c>
-      <c r="E33" s="29" t="s">
+      <c r="E33" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="F33" s="29" t="s">
+      <c r="F33" s="8" t="s">
         <v>70</v>
       </c>
-      <c r="G33" s="30" t="s">
+      <c r="G33" s="9" t="s">
         <v>69</v>
       </c>
-      <c r="H33" s="30" t="s">
+      <c r="H33" s="9" t="s">
         <v>32</v>
       </c>
       <c r="I33" s="2"/>
@@ -4129,28 +4118,28 @@
       <c r="Y33" s="1"/>
     </row>
     <row r="34" spans="1:25" ht="105" x14ac:dyDescent="0.2">
-      <c r="A34" s="28">
+      <c r="A34" s="13">
         <v>29</v>
       </c>
-      <c r="B34" s="29" t="s">
+      <c r="B34" s="8" t="s">
         <v>111</v>
       </c>
-      <c r="C34" s="29" t="s">
+      <c r="C34" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="D34" s="29" t="s">
+      <c r="D34" s="8" t="s">
         <v>110</v>
       </c>
-      <c r="E34" s="29" t="s">
+      <c r="E34" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="F34" s="29" t="s">
+      <c r="F34" s="8" t="s">
         <v>70</v>
       </c>
-      <c r="G34" s="30" t="s">
+      <c r="G34" s="9" t="s">
         <v>69</v>
       </c>
-      <c r="H34" s="30" t="s">
+      <c r="H34" s="9" t="s">
         <v>32</v>
       </c>
       <c r="I34" s="2"/>
@@ -4172,16 +4161,16 @@
       <c r="Y34" s="1"/>
     </row>
     <row r="35" spans="1:25" ht="33.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="18" t="s">
+      <c r="A35" s="26" t="s">
         <v>109</v>
       </c>
-      <c r="B35" s="15"/>
-      <c r="C35" s="15"/>
-      <c r="D35" s="15"/>
-      <c r="E35" s="15"/>
-      <c r="F35" s="15"/>
-      <c r="G35" s="15"/>
-      <c r="H35" s="14"/>
+      <c r="B35" s="24"/>
+      <c r="C35" s="24"/>
+      <c r="D35" s="24"/>
+      <c r="E35" s="24"/>
+      <c r="F35" s="24"/>
+      <c r="G35" s="24"/>
+      <c r="H35" s="25"/>
       <c r="I35" s="2"/>
       <c r="J35" s="1"/>
       <c r="K35" s="1"/>
@@ -4201,16 +4190,16 @@
       <c r="Y35" s="1"/>
     </row>
     <row r="36" spans="1:25" ht="33" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="16" t="s">
+      <c r="A36" s="23" t="s">
         <v>108</v>
       </c>
-      <c r="B36" s="15"/>
-      <c r="C36" s="15"/>
-      <c r="D36" s="15"/>
-      <c r="E36" s="15"/>
-      <c r="F36" s="15"/>
-      <c r="G36" s="15"/>
-      <c r="H36" s="14"/>
+      <c r="B36" s="24"/>
+      <c r="C36" s="24"/>
+      <c r="D36" s="24"/>
+      <c r="E36" s="24"/>
+      <c r="F36" s="24"/>
+      <c r="G36" s="24"/>
+      <c r="H36" s="25"/>
       <c r="I36" s="2"/>
       <c r="J36" s="1"/>
       <c r="K36" s="1"/>
@@ -4292,7 +4281,7 @@
       <c r="G38" s="9" t="s">
         <v>74</v>
       </c>
-      <c r="H38" s="17"/>
+      <c r="H38" s="14"/>
       <c r="I38" s="2"/>
       <c r="J38" s="1"/>
       <c r="K38" s="1"/>
@@ -4333,7 +4322,7 @@
       <c r="G39" s="9" t="s">
         <v>74</v>
       </c>
-      <c r="H39" s="17"/>
+      <c r="H39" s="14"/>
       <c r="I39" s="2"/>
       <c r="J39" s="1"/>
       <c r="K39" s="1"/>
@@ -4458,7 +4447,7 @@
       <c r="G42" s="9" t="s">
         <v>74</v>
       </c>
-      <c r="H42" s="17"/>
+      <c r="H42" s="14"/>
       <c r="I42" s="2"/>
       <c r="J42" s="1"/>
       <c r="K42" s="1"/>
@@ -4542,7 +4531,7 @@
       <c r="G44" s="9" t="s">
         <v>74</v>
       </c>
-      <c r="H44" s="17"/>
+      <c r="H44" s="14"/>
       <c r="I44" s="2"/>
       <c r="J44" s="1"/>
       <c r="K44" s="1"/>
@@ -4583,7 +4572,7 @@
       <c r="G45" s="9" t="s">
         <v>74</v>
       </c>
-      <c r="H45" s="17"/>
+      <c r="H45" s="14"/>
       <c r="I45" s="2"/>
       <c r="J45" s="1"/>
       <c r="K45" s="1"/>
@@ -4624,7 +4613,7 @@
       <c r="G46" s="9" t="s">
         <v>74</v>
       </c>
-      <c r="H46" s="17"/>
+      <c r="H46" s="14"/>
       <c r="I46" s="2"/>
       <c r="J46" s="1"/>
       <c r="K46" s="1"/>
@@ -4665,7 +4654,7 @@
       <c r="G47" s="9" t="s">
         <v>74</v>
       </c>
-      <c r="H47" s="17"/>
+      <c r="H47" s="14"/>
       <c r="I47" s="2"/>
       <c r="J47" s="1"/>
       <c r="K47" s="1"/>
@@ -4706,7 +4695,7 @@
       <c r="G48" s="9" t="s">
         <v>74</v>
       </c>
-      <c r="H48" s="17"/>
+      <c r="H48" s="14"/>
       <c r="I48" s="2"/>
       <c r="J48" s="1"/>
       <c r="K48" s="1"/>
@@ -4726,16 +4715,16 @@
       <c r="Y48" s="1"/>
     </row>
     <row r="49" spans="1:25" ht="36.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="16" t="s">
+      <c r="A49" s="23" t="s">
         <v>78</v>
       </c>
-      <c r="B49" s="15"/>
-      <c r="C49" s="15"/>
-      <c r="D49" s="15"/>
-      <c r="E49" s="15"/>
-      <c r="F49" s="15"/>
-      <c r="G49" s="15"/>
-      <c r="H49" s="14"/>
+      <c r="B49" s="24"/>
+      <c r="C49" s="24"/>
+      <c r="D49" s="24"/>
+      <c r="E49" s="24"/>
+      <c r="F49" s="24"/>
+      <c r="G49" s="24"/>
+      <c r="H49" s="25"/>
       <c r="I49" s="2"/>
       <c r="J49" s="1"/>
       <c r="K49" s="1"/>
@@ -30467,60 +30456,60 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:25" ht="29" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="21" t="s">
         <v>176</v>
       </c>
-      <c r="B1" s="27" t="s">
+      <c r="B1" s="21" t="s">
         <v>177</v>
       </c>
-      <c r="C1" s="27" t="s">
+      <c r="C1" s="21" t="s">
         <v>178</v>
       </c>
-      <c r="D1" s="27" t="s">
+      <c r="D1" s="21" t="s">
         <v>182</v>
       </c>
-      <c r="E1" s="27" t="s">
+      <c r="E1" s="21" t="s">
         <v>174</v>
       </c>
-      <c r="F1" s="27" t="s">
+      <c r="F1" s="21" t="s">
         <v>179</v>
       </c>
-      <c r="G1" s="27" t="s">
+      <c r="G1" s="21" t="s">
         <v>180</v>
       </c>
-      <c r="H1" s="27" t="s">
+      <c r="H1" s="21" t="s">
         <v>181</v>
       </c>
-      <c r="I1" s="27" t="s">
+      <c r="I1" s="21" t="s">
         <v>183</v>
       </c>
     </row>
     <row r="2" spans="1:25" ht="105" x14ac:dyDescent="0.2">
-      <c r="A2" s="22" t="s">
+      <c r="A2" s="16" t="s">
         <v>68</v>
       </c>
-      <c r="B2" s="22" t="s">
+      <c r="B2" s="16" t="s">
         <v>67</v>
       </c>
-      <c r="C2" s="23" t="s">
+      <c r="C2" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="24" t="s">
+      <c r="D2" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="25" t="s">
+      <c r="E2" s="19" t="s">
         <v>62</v>
       </c>
-      <c r="F2" s="25" t="s">
+      <c r="F2" s="19" t="s">
         <v>66</v>
       </c>
-      <c r="G2" s="25" t="s">
+      <c r="G2" s="19" t="s">
         <v>51</v>
       </c>
-      <c r="H2" s="22" t="s">
+      <c r="H2" s="16" t="s">
         <v>50</v>
       </c>
-      <c r="I2" s="26" t="s">
+      <c r="I2" s="20" t="s">
         <v>65</v>
       </c>
       <c r="J2" s="4"/>

</xml_diff>

<commit_message>
refactor: edit some titles
</commit_message>
<xml_diff>
--- a/yandex-samokat/yandex-samokat (mobile version).xlsx
+++ b/yandex-samokat/yandex-samokat (mobile version).xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vladefremov/Documents/Тестирование/ЯндексПрактикум/Practicum_projects/yandex-samokat/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58FC8B01-0CF7-4D45-ACD7-C380FD97E094}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BB5D002-C032-A843-B79C-C967CD6D94C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{D0BC9613-3873-3245-A71C-614316A097B5}"/>
+    <workbookView xWindow="28960" yWindow="-1460" windowWidth="38080" windowHeight="20780" activeTab="1" xr2:uid="{D0BC9613-3873-3245-A71C-614316A097B5}"/>
   </bookViews>
   <sheets>
     <sheet name="Тест-кейсы" sheetId="1" r:id="rId1"/>
@@ -2023,7 +2023,7 @@
     <t>Статус</t>
   </si>
   <si>
-    <t>Скрины/скринкасты</t>
+    <t>Приложения</t>
   </si>
 </sst>
 </file>
@@ -2768,8 +2768,8 @@
   </sheetPr>
   <dimension ref="A1:Y998"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
@@ -30438,9 +30438,9 @@
   </sheetPr>
   <dimension ref="A1:Y957"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J6" sqref="J6"/>
+    <sheetView tabSelected="1" zoomScale="118" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="15.19921875" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>